<commit_message>
add 服务器列表 and update db field
</commit_message>
<xml_diff>
--- a/doc/系统字段定义20180327.xlsx
+++ b/doc/系统字段定义20180327.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="设备基础信息" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="227">
   <si>
     <t>字段名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -272,12 +272,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>售后服务供应商电话</t>
-  </si>
-  <si>
-    <t>售后服务供应商描述</t>
-  </si>
-  <si>
     <t>使用状态</t>
   </si>
   <si>
@@ -287,19 +281,535 @@
     <t>是否在手机端必填</t>
   </si>
   <si>
-    <t>销售供应商联系人</t>
-  </si>
-  <si>
-    <t>销售供应商电话</t>
-  </si>
-  <si>
-    <t>销售供应商描述</t>
+    <t>保修合同结束时间</t>
+  </si>
+  <si>
+    <t>设备附件</t>
+  </si>
+  <si>
+    <t>设备负责人</t>
+  </si>
+  <si>
+    <t>维修手册</t>
+  </si>
+  <si>
+    <t>上传资料1</t>
+  </si>
+  <si>
+    <t>上传资料2</t>
+  </si>
+  <si>
+    <t>上传资料描述</t>
+  </si>
+  <si>
+    <t>上传资料3</t>
+  </si>
+  <si>
+    <t>上传资料4</t>
+  </si>
+  <si>
+    <t>纸质文件内容描述</t>
+  </si>
+  <si>
+    <t>用户手册</t>
+  </si>
+  <si>
+    <t>合同名称</t>
+  </si>
+  <si>
+    <t>1有、0没有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1使用、0停用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售供应商名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HospitalId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DepartmentId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Picture1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Picture2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Picture3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Picture4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Picture5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AssetNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceModel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1正常、2故障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B超，MR，普放等等（字典值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SerialNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UsageState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QRCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProducingPlace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accessory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetupDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AcceptDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AcceptRemark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AcceptFile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UseDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StorageDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>采购金额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PurchaseAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保修期结束时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaintenanceEndDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WarrantyBeginDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WarrantyEndDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WarrantyAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>保</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>修合同内容</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WarrantyContent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SalesSupplier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SalesSupplierContact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SalesSupplierPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SalesSupplierDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>售后服务供应商名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AfterSaleProvider</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AfterSaleProviderEngineer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AfterSaleProviderPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AfterSaleProviderDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ContractId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ModifyTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creater</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserManual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaintenanceManual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简易使用手册</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Handbook</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data1Desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data2Desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data3Desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data4Desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>纸质文件存放地点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaperFileContent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaperFilePlace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ContractNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ContractName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ContractFile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>采购负责人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PurchaseId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否招标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HasBid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1是，0否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PurchaseOwner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceOwner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HospitalId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HospitalName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HospitalAddr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AreaId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeptId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeptName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeptOwner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ParentDeptId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AreaId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>行政编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>父区域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ParentId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AreaType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天气编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AreaName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdminCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮政编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WeatherCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关系ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RelId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoginPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mobile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DisplayName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoginName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HospitalId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HospitalId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>保修合同开始时间</t>
-  </si>
-  <si>
-    <t>保修合同结束时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -322,504 +832,58 @@
       </rPr>
       <t>修合同金额</t>
     </r>
-  </si>
-  <si>
-    <t>设备附件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售供应商联系人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售供应商电话</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售供应商描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>售后服务供应商工程师</t>
-  </si>
-  <si>
-    <t>设备负责人</t>
-  </si>
-  <si>
-    <t>维修手册</t>
-  </si>
-  <si>
-    <t>上传资料1</t>
-  </si>
-  <si>
-    <t>上传资料2</t>
-  </si>
-  <si>
-    <t>上传资料描述</t>
-  </si>
-  <si>
-    <t>上传资料3</t>
-  </si>
-  <si>
-    <t>上传资料4</t>
-  </si>
-  <si>
-    <t>纸质文件内容描述</t>
-  </si>
-  <si>
-    <t>用户手册</t>
-  </si>
-  <si>
-    <t>合同名称</t>
-  </si>
-  <si>
-    <t>1有、0没有</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1使用、0停用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>销售供应商名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HospitalId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DepartmentId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Picture1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Picture2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Picture3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Picture4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Picture5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AssetNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceModel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceDesc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceState</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1正常、2故障</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B超，MR，普放等等（字典值）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SerialNumber</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UsageState</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>QRCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ProducingPlace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Accessory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SetupDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AcceptDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AcceptRemark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AcceptFile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UseDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StorageDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>采购金额</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PurchaseAmount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>保修期结束时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MaintenanceEndDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WarrantyBeginDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WarrantyEndDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WarrantyAmount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>保</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>修合同内容</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WarrantyContent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SalesSupplier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SalesSupplierContact</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SalesSupplierPhone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SalesSupplierDesc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>售后服务供应商名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AfterSaleProvider</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AfterSaleProviderEngineer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AfterSaleProviderPhone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AfterSaleProviderDesc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ContractId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreateTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modifier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ModifyTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creater</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserManual</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MaintenanceManual</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>简易使用手册</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Handbook</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data1Desc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data2Desc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data3Desc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data4Desc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>纸质文件存放地点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PaperFileContent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PaperFilePlace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ContractNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ContractName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ContractFile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>采购负责人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PurchaseId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否招标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HasBid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1是，0否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PurchaseOwner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeviceOwner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HospitalId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HospitalName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HospitalAddr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AreaId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeptId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeptName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeptOwner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ParentDeptId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>区域Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AreaId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>行政编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>区域名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>区域类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>父区域</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ParentId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AreaType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10:国家，20：省，30：市，40：区县</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>天气编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AreaName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AdminCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PostCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>邮政编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WeatherCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>邮箱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登录名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>售后服务供应商电话</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>售后服务供应商描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合同ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10：国家，30：省，50，市；70：县，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZipCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国家编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountryCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域深度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AreaDepth</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -827,59 +891,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>关系ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RelId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LoginPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mobile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DisplayName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LoginName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HospitalId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HospitalId</t>
+    <t>区域路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AreaPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeptPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部门路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传资料5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data5Desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AccessoryId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data1File</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data2File</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data3File</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data4File</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data5File</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -972,6 +1048,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -991,7 +1135,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1026,7 +1170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1058,9 +1202,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1092,6 +1237,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1267,14 +1413,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:D52"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.25" customWidth="1"/>
     <col min="2" max="2" width="28.25" bestFit="1" customWidth="1"/>
@@ -1286,7 +1432,7 @@
     <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1306,48 +1452,48 @@
         <v>53</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
         <v>50</v>
@@ -1356,15 +1502,15 @@
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
@@ -1373,516 +1519,516 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
         <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
         <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>196</v>
       </c>
       <c r="B33" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>197</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" t="s">
         <v>125</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" t="s">
         <v>126</v>
       </c>
-      <c r="D36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="D44" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B45" t="s">
         <v>127</v>
       </c>
-      <c r="D38" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" t="s">
         <v>128</v>
-      </c>
-      <c r="D39" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" t="s">
-        <v>129</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" t="s">
-        <v>132</v>
-      </c>
-      <c r="D42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" t="s">
-        <v>133</v>
-      </c>
-      <c r="D43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" t="s">
-        <v>135</v>
-      </c>
-      <c r="D45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" t="s">
-        <v>136</v>
       </c>
       <c r="C47" t="s">
         <v>48</v>
@@ -1891,45 +2037,45 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D49" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D51" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D52" t="s">
         <v>21</v>
@@ -1967,16 +2113,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1984,7 +2130,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1992,22 +2138,22 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2019,21 +2165,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2047,209 +2194,245 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>220</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>86</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>144</v>
+        <v>69</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>149</v>
+        <v>222</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>150</v>
+        <v>223</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>151</v>
+        <v>224</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>152</v>
+        <v>225</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>153</v>
+        <v>72</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>83</v>
+        <v>218</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>154</v>
+        <v>226</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2264,13 +2447,13 @@
           <x14:formula1>
             <xm:f>序列!$A$2:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>D21:D76 D5:D16</xm:sqref>
+          <xm:sqref>D24:D79 D6:D19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>序列!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D17:D20 D2:D4</xm:sqref>
+          <xm:sqref>D20:D23 D2:D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2279,21 +2462,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.125" customWidth="1"/>
     <col min="2" max="2" width="35.75" customWidth="1"/>
     <col min="3" max="3" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2307,123 +2490,123 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
@@ -2454,21 +2637,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.625" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="28.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2482,92 +2665,92 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
@@ -2598,20 +2781,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.375" customWidth="1"/>
     <col min="4" max="4" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2625,48 +2810,92 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2689,14 +2918,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.375" customWidth="1"/>
     <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
@@ -2704,7 +2933,7 @@
     <col min="4" max="4" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2718,100 +2947,122 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -2836,14 +3087,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
@@ -2851,7 +3102,7 @@
     <col min="4" max="4" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2865,111 +3116,111 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
         <v>190</v>
       </c>
-      <c r="B2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
         <v>191</v>
       </c>
-      <c r="B4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" t="s">
         <v>192</v>
       </c>
-      <c r="B5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B7" t="s">
-        <v>206</v>
-      </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
@@ -2982,20 +3233,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.375" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3009,78 +3260,78 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
@@ -3094,21 +3345,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3122,125 +3373,158 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -3249,5 +3533,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="96" verticalDpi="96" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>